<commit_message>
Sounds and some tweaks
</commit_message>
<xml_diff>
--- a/pinball/docs/Arduino pins.xlsx
+++ b/pinball/docs/Arduino pins.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="1545" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2C5C205-BC47-4DA6-BE6A-D5799B895BBC}"/>
+  <xr:revisionPtr revIDLastSave="1547" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2905C8AD-D86B-419F-8B78-4BEBE93F5F68}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pinball" sheetId="3" r:id="rId1"/>
@@ -28,255 +28,261 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="147">
+  <si>
+    <t>"Master" Arduino</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>D/A</t>
+  </si>
+  <si>
+    <t>Port</t>
+  </si>
+  <si>
+    <t>Connected</t>
+  </si>
+  <si>
+    <t>leftButton</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>rightButton</t>
+  </si>
+  <si>
+    <t>D3 ~</t>
+  </si>
+  <si>
+    <t>leftOutlaneSensor</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
+    <t>rightOutlaneSensor</t>
+  </si>
+  <si>
+    <t>D5 ~</t>
+  </si>
+  <si>
+    <t>rolloverSkillSensor</t>
+  </si>
+  <si>
+    <t>D6 ~</t>
+  </si>
+  <si>
+    <t>rollover3Sensor</t>
+  </si>
+  <si>
+    <t>D7</t>
+  </si>
+  <si>
+    <t>rollover2Sensor</t>
+  </si>
+  <si>
+    <t>D8</t>
+  </si>
+  <si>
+    <t>rollover1Sensor</t>
+  </si>
+  <si>
+    <t>D9 ~</t>
+  </si>
+  <si>
+    <t>leftFlipper</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>L298N (19V)</t>
+  </si>
+  <si>
+    <t>IN2</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>D10 ~</t>
+  </si>
+  <si>
+    <t>rightFlipper</t>
+  </si>
+  <si>
+    <t>IN1</t>
+  </si>
+  <si>
+    <t>D11 ~</t>
+  </si>
+  <si>
+    <t>ballLostSensor</t>
+  </si>
+  <si>
+    <t>D12</t>
+  </si>
+  <si>
+    <t>stopMagnet</t>
+  </si>
+  <si>
+    <t>DRV8833 (9V)</t>
+  </si>
+  <si>
+    <t>In4</t>
+  </si>
+  <si>
+    <t>D13</t>
+  </si>
+  <si>
+    <t>feederHomeSensor</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>ballNearHomeSensor</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>spinnerSensor</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>leftOrbitSensor</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>holdSensor</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>launchSensor</t>
+  </si>
+  <si>
+    <t>A7</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>"Child" Arduino</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>soundTx</t>
+  </si>
+  <si>
+    <t>via 1 kohm</t>
+  </si>
+  <si>
+    <t>soundRx</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>unused</t>
+  </si>
+  <si>
+    <t>doorServo</t>
+  </si>
+  <si>
+    <t>feederMotor</t>
+  </si>
+  <si>
+    <t>In3</t>
+  </si>
+  <si>
+    <t>rolloverSkillLed</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>rollover3Led</t>
+  </si>
+  <si>
+    <t>rollover2Led</t>
+  </si>
+  <si>
+    <t>rollover1Led</t>
+  </si>
+  <si>
+    <t>Lights</t>
+  </si>
+  <si>
+    <t>In2</t>
+  </si>
+  <si>
+    <t>leftOrbitLed</t>
+  </si>
+  <si>
+    <t>holdLed</t>
+  </si>
+  <si>
+    <t>leftOutlaneLed</t>
+  </si>
+  <si>
+    <t>rightOutlaneLed</t>
+  </si>
   <si>
     <t>Arduino 1</t>
   </si>
   <si>
-    <t>I/O</t>
-  </si>
-  <si>
-    <t>Driver</t>
-  </si>
-  <si>
-    <t>Pin</t>
-  </si>
-  <si>
-    <t>D/A</t>
-  </si>
-  <si>
-    <t>Port</t>
-  </si>
-  <si>
-    <t>Connected</t>
-  </si>
-  <si>
-    <t>leftButton</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>rightButton</t>
-  </si>
-  <si>
-    <t>D3 ~</t>
-  </si>
-  <si>
-    <t>leftOutlaneSensor</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>rightOutlaneSensor</t>
-  </si>
-  <si>
-    <t>D5 ~</t>
-  </si>
-  <si>
-    <t>rolloverSkillSensor</t>
-  </si>
-  <si>
-    <t>D6 ~</t>
-  </si>
-  <si>
-    <t>rollover3Sensor</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>rollover2Sensor</t>
-  </si>
-  <si>
-    <t>D8</t>
-  </si>
-  <si>
-    <t>rollover1Sensor</t>
-  </si>
-  <si>
-    <t>D9 ~</t>
-  </si>
-  <si>
-    <t>leftFlipper</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>L298N (19V)</t>
-  </si>
-  <si>
-    <t>IN2</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>D10 ~</t>
-  </si>
-  <si>
-    <t>rightFlipper</t>
-  </si>
-  <si>
-    <t>IN1</t>
-  </si>
-  <si>
-    <t>D11 ~</t>
-  </si>
-  <si>
-    <t>ballLostSensor</t>
-  </si>
-  <si>
-    <t>D12</t>
-  </si>
-  <si>
-    <t>stopMagnet</t>
-  </si>
-  <si>
-    <t>DRV8833 (9V)</t>
-  </si>
-  <si>
-    <t>In4</t>
-  </si>
-  <si>
-    <t>D13</t>
-  </si>
-  <si>
-    <t>feederHomeSensor</t>
-  </si>
-  <si>
-    <t>A0</t>
-  </si>
-  <si>
-    <t>ballNearHomeSensor</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>spinnerSensor</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>leftOrbitSensor</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>SDA</t>
-  </si>
-  <si>
-    <t>green</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>SCL</t>
-  </si>
-  <si>
-    <t>blue</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
-    <t>holdSensor</t>
-  </si>
-  <si>
-    <t>A6</t>
-  </si>
-  <si>
-    <t>launchSensor</t>
-  </si>
-  <si>
-    <t>A7</t>
-  </si>
-  <si>
-    <t>reset</t>
-  </si>
-  <si>
-    <t>Reset</t>
-  </si>
-  <si>
     <t>Arduino 2</t>
-  </si>
-  <si>
-    <t>PWM</t>
-  </si>
-  <si>
-    <t>soundTx</t>
-  </si>
-  <si>
-    <t>via 1 kohm</t>
-  </si>
-  <si>
-    <t>soundRx</t>
-  </si>
-  <si>
-    <t>Direct</t>
-  </si>
-  <si>
-    <t>unused</t>
-  </si>
-  <si>
-    <t>doorServo</t>
-  </si>
-  <si>
-    <t>feederMotor</t>
-  </si>
-  <si>
-    <t>In3</t>
-  </si>
-  <si>
-    <t>rolloverSkillLed</t>
-  </si>
-  <si>
-    <t>5V</t>
-  </si>
-  <si>
-    <t>rollover3Led</t>
-  </si>
-  <si>
-    <t>rollover2Led</t>
-  </si>
-  <si>
-    <t>rollover1Led</t>
-  </si>
-  <si>
-    <t>Lights</t>
-  </si>
-  <si>
-    <t>In2</t>
-  </si>
-  <si>
-    <t>leftOrbitLed</t>
-  </si>
-  <si>
-    <t>holdLed</t>
-  </si>
-  <si>
-    <t>leftOutlaneLed</t>
-  </si>
-  <si>
-    <t>rightOutlaneLed</t>
   </si>
   <si>
     <t>rgbPixelsPin</t>
@@ -1015,9 +1021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0614AC0C-A919-4420-A2E4-FD05D0056BB8}">
   <dimension ref="B1:I48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1877,7 +1883,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A7B114-6970-4D73-A29F-5FAA679B88A2}">
   <dimension ref="B1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
     </sheetView>
@@ -1897,7 +1903,7 @@
   <sheetData>
     <row r="1" spans="2:9" ht="24.75" customHeight="1">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
@@ -2311,7 +2317,7 @@
     </row>
     <row r="25" spans="2:9">
       <c r="B25" s="1" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>1</v>
@@ -2614,7 +2620,7 @@
     </row>
     <row r="42" spans="2:9">
       <c r="B42" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>30</v>
@@ -2745,10 +2751,10 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>1</v>
@@ -2766,10 +2772,10 @@
     </row>
     <row r="4" spans="2:7">
       <c r="B4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -2783,10 +2789,10 @@
     </row>
     <row r="5" spans="2:7">
       <c r="B5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>8</v>
@@ -2800,10 +2806,10 @@
     </row>
     <row r="6" spans="2:7">
       <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -2817,10 +2823,10 @@
     </row>
     <row r="7" spans="2:7">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>8</v>
@@ -2834,10 +2840,10 @@
     </row>
     <row r="8" spans="2:7">
       <c r="B8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>8</v>
@@ -2851,10 +2857,10 @@
     </row>
     <row r="9" spans="2:7">
       <c r="B9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
@@ -2868,10 +2874,10 @@
     </row>
     <row r="10" spans="2:7">
       <c r="B10" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>8</v>
@@ -2885,10 +2891,10 @@
     </row>
     <row r="11" spans="2:7">
       <c r="B11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>8</v>
@@ -2902,10 +2908,10 @@
     </row>
     <row r="12" spans="2:7">
       <c r="B12" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>8</v>
@@ -2919,10 +2925,10 @@
     </row>
     <row r="13" spans="2:7">
       <c r="B13" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>8</v>
@@ -2936,10 +2942,10 @@
     </row>
     <row r="14" spans="2:7">
       <c r="B14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>8</v>
@@ -2953,7 +2959,7 @@
     </row>
     <row r="15" spans="2:7">
       <c r="B15" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>27</v>
@@ -2967,10 +2973,10 @@
     </row>
     <row r="16" spans="2:7">
       <c r="B16" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
@@ -2985,10 +2991,10 @@
     </row>
     <row r="17" spans="2:12">
       <c r="B17" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
@@ -3002,10 +3008,10 @@
     </row>
     <row r="18" spans="2:12">
       <c r="B18" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>8</v>
@@ -3019,10 +3025,10 @@
     </row>
     <row r="19" spans="2:12">
       <c r="B19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>8</v>
@@ -3039,7 +3045,7 @@
         <v>50</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>1</v>
@@ -3058,7 +3064,7 @@
         <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>1</v>
@@ -3072,10 +3078,10 @@
     </row>
     <row r="22" spans="2:12">
       <c r="B22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>8</v>
@@ -3090,10 +3096,10 @@
     </row>
     <row r="23" spans="2:12">
       <c r="B23" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -3111,7 +3117,7 @@
     </row>
     <row r="25" spans="2:12">
       <c r="B25" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="3" t="s">
@@ -3128,21 +3134,21 @@
       <c r="C26" s="2"/>
       <c r="I26" s="12"/>
       <c r="J26" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="L26" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="2:12">
       <c r="B27" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>27</v>
@@ -3160,10 +3166,10 @@
     </row>
     <row r="28" spans="2:12">
       <c r="B28" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>27</v>
@@ -3175,19 +3181,19 @@
         <v>13</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I28" s="12"/>
       <c r="J28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="2:12">
       <c r="B29" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>30</v>
@@ -3198,18 +3204,18 @@
       <c r="H29" s="8"/>
       <c r="I29" s="12"/>
       <c r="J29" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="30" spans="2:12">
       <c r="B30" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>27</v>
@@ -3221,22 +3227,22 @@
         <v>17</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I30" s="12"/>
       <c r="J30" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="2:12">
       <c r="B31" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>27</v>
@@ -3252,18 +3258,18 @@
       </c>
       <c r="I31" s="12"/>
       <c r="J31" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="2:12">
       <c r="B32" s="4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>27</v>
@@ -3279,18 +3285,18 @@
       </c>
       <c r="I32" s="12"/>
       <c r="J32" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="2:11">
       <c r="B33" s="4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>27</v>
@@ -3306,18 +3312,18 @@
       </c>
       <c r="I33" s="12"/>
       <c r="J33" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K33" s="10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="2:11">
       <c r="B34" s="4" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>27</v>
@@ -3333,18 +3339,18 @@
       </c>
       <c r="I34" s="12"/>
       <c r="J34" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="2:11">
       <c r="B35" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>27</v>
@@ -3356,22 +3362,22 @@
         <v>31</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I35" s="12"/>
       <c r="J35" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="2:11">
       <c r="B36" s="4" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>27</v>
@@ -3389,7 +3395,7 @@
     </row>
     <row r="37" spans="2:11">
       <c r="B37" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>30</v>
@@ -3400,15 +3406,15 @@
       <c r="H37" s="8"/>
       <c r="I37" s="12"/>
       <c r="J37" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="2:11">
       <c r="B38" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>27</v>
@@ -3426,7 +3432,7 @@
     </row>
     <row r="39" spans="2:11">
       <c r="B39" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>27</v>
@@ -3439,18 +3445,18 @@
       </c>
       <c r="I39" s="12"/>
       <c r="J39" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K39" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="2:11">
       <c r="B40" s="7" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>27</v>
@@ -3466,18 +3472,18 @@
       </c>
       <c r="I40" s="12"/>
       <c r="J40" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K40" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="2:11">
       <c r="B41" s="7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>27</v>
@@ -3493,18 +3499,18 @@
       </c>
       <c r="I41" s="12"/>
       <c r="J41" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K41" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="2:11">
       <c r="B42" s="7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>27</v>
@@ -3520,10 +3526,10 @@
       </c>
       <c r="I42" s="12"/>
       <c r="J42" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="K42" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="2:11">
@@ -3531,7 +3537,7 @@
         <v>50</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>1</v>
@@ -3544,10 +3550,10 @@
       </c>
       <c r="I43" s="12"/>
       <c r="J43" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K43" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="2:11">
@@ -3555,7 +3561,7 @@
         <v>53</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>1</v>
@@ -3568,15 +3574,15 @@
       </c>
       <c r="I44" s="12"/>
       <c r="J44" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K44" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="2:11">
       <c r="B45" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C45" s="2"/>
       <c r="E45" s="2" t="s">
@@ -3587,15 +3593,15 @@
       </c>
       <c r="I45" s="12"/>
       <c r="J45" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K45" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="2:11">
       <c r="B46" s="14" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C46" s="2"/>
       <c r="E46" s="2" t="s">
@@ -3606,10 +3612,10 @@
       </c>
       <c r="I46" s="12"/>
       <c r="J46" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K46" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>